<commit_message>
switch to Quarto - big changes 3
</commit_message>
<xml_diff>
--- a/tabellen/Tabel_Dendro_veldatum.xlsx
+++ b/tabellen/Tabel_Dendro_veldatum.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\handleidingDendro\tabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359B4653-5923-460C-A79C-73E4FDBCAF58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785CBD94-E278-4566-8A99-4F795FACFB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BFFEBC10-6255-4FAB-8BFC-808908C657BC}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>Einddatering</t>
   </si>
   <si>
-    <t>Schatting ontbrekend spint</t>
-  </si>
-  <si>
     <t>Veldatum</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Aantal ringen</t>
   </si>
   <si>
-    <t>Spinthoutringen</t>
-  </si>
-  <si>
     <t>NOV-14</t>
   </si>
   <si>
@@ -171,10 +165,16 @@
     <t>NOV-22</t>
   </si>
   <si>
-    <t>Schors/wankant*</t>
-  </si>
-  <si>
     <t>WK</t>
+  </si>
+  <si>
+    <t>Schors/ wankant</t>
+  </si>
+  <si>
+    <t>Ontbrekend spint</t>
+  </si>
+  <si>
+    <t>Spinthout- ringen</t>
   </si>
 </sst>
 </file>
@@ -530,7 +530,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,22 +548,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -580,10 +580,10 @@
         <v>1294</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -597,10 +597,10 @@
         <v>1279</v>
       </c>
       <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -617,10 +617,10 @@
         <v>1285</v>
       </c>
       <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
         <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -637,10 +637,10 @@
         <v>1285</v>
       </c>
       <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
         <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -657,10 +657,10 @@
         <v>1277</v>
       </c>
       <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
         <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -677,10 +677,10 @@
         <v>1284</v>
       </c>
       <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
         <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -694,10 +694,10 @@
         <v>1239</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -711,10 +711,10 @@
         <v>1232</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -728,21 +728,21 @@
         <v>1211</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <v>19</v>
@@ -751,12 +751,12 @@
         <v>1271</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>114</v>
@@ -768,15 +768,15 @@
         <v>1269</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>104</v>
@@ -785,15 +785,15 @@
         <v>1253</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>116</v>
@@ -805,15 +805,15 @@
         <v>1260</v>
       </c>
       <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
         <v>31</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>61</v>
@@ -825,21 +825,21 @@
         <v>1247</v>
       </c>
       <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
         <v>33</v>
-      </c>
-      <c r="G15" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>127</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16">
         <v>18</v>
@@ -848,12 +848,12 @@
         <v>1289</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>66</v>
@@ -862,10 +862,10 @@
         <v>1257</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>